<commit_message>
login, logout, formendingtests added
</commit_message>
<xml_diff>
--- a/Software quality and testing - Selenium assignment.xlsx
+++ b/Software quality and testing - Selenium assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\selenium-docker-sandbox\tests\selenium-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F3E98-001C-4DED-81B0-D3B0E1D1510F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE24700-2C51-4D5F-A9AD-09F6FAEE08CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="57">
   <si>
     <t>This spreadsheet just a help tool to follow your done tasks, but this is only a calculator, on presentation the points can be lowered.</t>
   </si>
@@ -730,7 +730,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -845,7 +845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -871,12 +871,12 @@
         <v>11</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1"/>
       <c r="M4" s="2">
         <f t="array" ref="M4">SUM(IF(J3:J44&lt;&gt;"",IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N4" s="2">
         <f t="array" ref="N4">SUM(IF((J3:J44&lt;&gt;"")*(B3:B44="A"),IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
@@ -909,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>13</v>
@@ -947,7 +947,7 @@
         <v>11</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="L6" s="1">
         <v>2</v>
@@ -1100,8 +1100,8 @@
       <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>56</v>
+      <c r="J11" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -1281,7 +1281,7 @@
         <v>11</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="M18" s="5"/>
     </row>
@@ -1374,7 +1374,7 @@
         <v>11</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
redesign and staticpage added
</commit_message>
<xml_diff>
--- a/Software quality and testing - Selenium assignment.xlsx
+++ b/Software quality and testing - Selenium assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\selenium-docker-sandbox\tests\selenium-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE24700-2C51-4D5F-A9AD-09F6FAEE08CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7CFA62-846B-408B-99EA-518667C94307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -876,7 +876,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="2">
         <f t="array" ref="M4">SUM(IF(J3:J44&lt;&gt;"",IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N4" s="2">
         <f t="array" ref="N4">SUM(IF((J3:J44&lt;&gt;"")*(B3:B44="A"),IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
@@ -1101,7 +1101,7 @@
         <v>11</v>
       </c>
       <c r="J11" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
multiple static page tests added
</commit_message>
<xml_diff>
--- a/Software quality and testing - Selenium assignment.xlsx
+++ b/Software quality and testing - Selenium assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\selenium-docker-sandbox\tests\selenium-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7CFA62-846B-408B-99EA-518667C94307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2B061B-56DD-4D4C-AD4C-5DBA8AD439C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,8 +138,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
   <si>
     <t>This spreadsheet just a help tool to follow your done tasks, but this is only a calculator, on presentation the points can be lowered.</t>
   </si>
@@ -308,9 +330,6 @@
   </si>
   <si>
     <t>https://github.com/balazsbalint7/selenium-assignment</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -730,7 +749,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -789,7 +808,7 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -876,7 +895,7 @@
       <c r="K4" s="1"/>
       <c r="M4" s="2">
         <f t="array" ref="M4">SUM(IF(J3:J44&lt;&gt;"",IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N4" s="2">
         <f t="array" ref="N4">SUM(IF((J3:J44&lt;&gt;"")*(B3:B44="A"),IF(ISNUMBER(J3:J44)*(C3:C44="Repeatable"),J3:J44*D3:D44,D3:D44),0))</f>
@@ -1040,7 +1059,7 @@
         <v>11</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="L9" s="1">
         <v>5</v>
@@ -1072,7 +1091,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -1101,7 +1120,7 @@
         <v>11</v>
       </c>
       <c r="J11" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
@@ -1200,12 +1219,12 @@
         <v>11</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="L15" s="1">
         <v>4</v>
       </c>
-      <c r="M15" s="11" t="str">
+      <c r="M15" s="11" t="str" cm="1">
         <f t="array" ref="M15">IF(SUM(IF(($G$3:$G$44&lt;&gt;"")*($J$3:$J$44=""),1,0)) = 0, "OK", "Not satisfied")</f>
         <v>OK</v>
       </c>
@@ -1230,7 +1249,7 @@
         <v>11</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="L16" s="1">
         <v>5</v>
@@ -1311,7 +1330,7 @@
         <v>11</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -1334,7 +1353,7 @@
         <v>11</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
@@ -1354,7 +1373,7 @@
         <v>11</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>